<commit_message>
Template for Clue Board
</commit_message>
<xml_diff>
--- a/Planning_Board_Spreadsheet.xlsx
+++ b/Planning_Board_Spreadsheet.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="18315" windowHeight="5070"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -64,9 +65,6 @@
     <t>K</t>
   </si>
   <si>
-    <t>KL</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -149,6 +147,9 @@
   </si>
   <si>
     <t>Starting position for #th character</t>
+  </si>
+  <si>
+    <t>KR</t>
   </si>
 </sst>
 </file>
@@ -541,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,37 +574,37 @@
         <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>6</v>
@@ -650,10 +651,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>2</v>
@@ -677,10 +678,10 @@
         <v>2</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>6</v>
@@ -707,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="AB2" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
@@ -737,10 +738,10 @@
         <v>0</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>2</v>
@@ -764,10 +765,10 @@
         <v>2</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>6</v>
@@ -794,7 +795,7 @@
         <v>2</v>
       </c>
       <c r="AB3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
@@ -824,10 +825,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>2</v>
@@ -851,10 +852,10 @@
         <v>2</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>6</v>
@@ -881,7 +882,7 @@
         <v>6</v>
       </c>
       <c r="AB4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
@@ -890,31 +891,31 @@
     </row>
     <row r="5" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>4</v>
@@ -938,10 +939,10 @@
         <v>2</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>6</v>
@@ -965,10 +966,10 @@
         <v>6</v>
       </c>
       <c r="AA5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AB5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
@@ -977,31 +978,31 @@
     </row>
     <row r="6" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>2</v>
@@ -1025,10 +1026,10 @@
         <v>2</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S6" s="6" t="s">
         <v>5</v>
@@ -1055,7 +1056,7 @@
         <v>9</v>
       </c>
       <c r="AB6" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
@@ -1064,31 +1065,31 @@
     </row>
     <row r="7" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>2</v>
@@ -1112,37 +1113,37 @@
         <v>2</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AA7" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AB7" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
@@ -1151,85 +1152,85 @@
     </row>
     <row r="8" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AA8" s="8" t="s">
         <v>15</v>
       </c>
       <c r="AB8" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
@@ -1238,85 +1239,85 @@
     </row>
     <row r="9" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AA9" s="8" t="s">
         <v>12</v>
       </c>
       <c r="AB9" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
@@ -1325,34 +1326,34 @@
     </row>
     <row r="10" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="H10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>14</v>
@@ -1373,7 +1374,7 @@
         <v>14</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>9</v>
@@ -1403,7 +1404,7 @@
         <v>10</v>
       </c>
       <c r="AB10" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
@@ -1412,34 +1413,34 @@
     </row>
     <row r="11" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>14</v>
@@ -1460,7 +1461,7 @@
         <v>14</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R11" s="2" t="s">
         <v>9</v>
@@ -1487,10 +1488,10 @@
         <v>9</v>
       </c>
       <c r="AA11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB11" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
@@ -1499,34 +1500,34 @@
     </row>
     <row r="12" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>14</v>
@@ -1547,7 +1548,7 @@
         <v>14</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>9</v>
@@ -1574,10 +1575,10 @@
         <v>9</v>
       </c>
       <c r="AA12" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AB12" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
@@ -1586,34 +1587,34 @@
     </row>
     <row r="13" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>14</v>
@@ -1634,7 +1635,7 @@
         <v>14</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R13" s="6" t="s">
         <v>8</v>
@@ -1664,7 +1665,7 @@
         <v>14</v>
       </c>
       <c r="AB13" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
@@ -1673,34 +1674,34 @@
     </row>
     <row r="14" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>14</v>
@@ -1721,7 +1722,7 @@
         <v>14</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R14" s="6" t="s">
         <v>8</v>
@@ -1748,10 +1749,10 @@
         <v>9</v>
       </c>
       <c r="AA14" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
@@ -1760,34 +1761,34 @@
     </row>
     <row r="15" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>14</v>
@@ -1808,7 +1809,7 @@
         <v>14</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R15" s="2" t="s">
         <v>9</v>
@@ -1837,34 +1838,34 @@
     </row>
     <row r="16" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>14</v>
@@ -1885,7 +1886,7 @@
         <v>14</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R16" s="2" t="s">
         <v>9</v>
@@ -1914,64 +1915,64 @@
     </row>
     <row r="17" spans="1:25" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U17" s="2" t="s">
         <v>9</v>
@@ -1991,31 +1992,31 @@
     </row>
     <row r="18" spans="1:25" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>12</v>
@@ -2042,57 +2043,57 @@
         <v>12</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Y18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A19" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>12</v>
@@ -2119,57 +2120,57 @@
         <v>12</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Y19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A20" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>12</v>
@@ -2196,10 +2197,10 @@
         <v>12</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T20" s="2" t="s">
         <v>10</v>
@@ -2217,7 +2218,7 @@
         <v>10</v>
       </c>
       <c r="Y20" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
@@ -2237,16 +2238,16 @@
         <v>15</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>12</v>
@@ -2273,10 +2274,10 @@
         <v>12</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T21" s="2" t="s">
         <v>10</v>
@@ -2320,10 +2321,10 @@
         <v>15</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>12</v>
@@ -2350,10 +2351,10 @@
         <v>12</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T22" s="2" t="s">
         <v>10</v>
@@ -2397,10 +2398,10 @@
         <v>15</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>12</v>
@@ -2427,10 +2428,10 @@
         <v>12</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T23" s="2" t="s">
         <v>10</v>
@@ -2474,16 +2475,16 @@
         <v>15</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>12</v>
@@ -2498,16 +2499,16 @@
         <v>12</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T24" s="2" t="s">
         <v>10</v>
@@ -2551,40 +2552,40 @@
         <v>15</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P25" s="5" t="s">
+      <c r="Q25" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Q25" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="R25" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T25" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
First set of her tests working.
</commit_message>
<xml_diff>
--- a/Planning_Board_Spreadsheet.xlsx
+++ b/Planning_Board_Spreadsheet.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="37">
   <si>
     <t>C</t>
   </si>
@@ -86,30 +85,6 @@
     <t>W</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>S3</t>
-  </si>
-  <si>
-    <t>S4</t>
-  </si>
-  <si>
-    <t>S5</t>
-  </si>
-  <si>
-    <t>S6</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>S#</t>
-  </si>
-  <si>
     <t>Conservatory</t>
   </si>
   <si>
@@ -146,10 +121,10 @@
     <t>Closet</t>
   </si>
   <si>
-    <t>Starting position for #th character</t>
-  </si>
-  <si>
     <t>KR</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -173,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,12 +181,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -229,14 +198,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -542,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +545,7 @@
         <v>22</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>2</v>
@@ -601,10 +569,10 @@
         <v>2</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>6</v>
@@ -704,11 +672,11 @@
       <c r="Y2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AA2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="8" t="s">
-        <v>31</v>
+      <c r="AA2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
@@ -791,11 +759,11 @@
       <c r="Y3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AA3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB3" s="8" t="s">
-        <v>32</v>
+      <c r="AA3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
@@ -821,7 +789,7 @@
       <c r="F4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -878,11 +846,11 @@
       <c r="Y4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AA4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB4" s="8" t="s">
-        <v>33</v>
+      <c r="AA4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB4" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
@@ -891,7 +859,7 @@
     </row>
     <row r="5" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>22</v>
@@ -917,7 +885,7 @@
       <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -965,11 +933,11 @@
       <c r="Y5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AA5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB5" s="8" t="s">
-        <v>34</v>
+      <c r="AA5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB5" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
@@ -977,8 +945,8 @@
       <c r="AF5" s="1"/>
     </row>
     <row r="6" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A6" s="5" t="s">
-        <v>25</v>
+      <c r="A6" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>22</v>
@@ -1031,7 +999,7 @@
       <c r="R6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="S6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="T6" s="2" t="s">
@@ -1052,11 +1020,11 @@
       <c r="Y6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AA6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB6" s="8" t="s">
-        <v>35</v>
+      <c r="AA6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
@@ -1100,10 +1068,10 @@
       <c r="L7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="N7" s="5" t="s">
         <v>3</v>
       </c>
       <c r="O7" s="2" t="s">
@@ -1137,13 +1105,13 @@
         <v>22</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB7" s="8" t="s">
         <v>36</v>
+      </c>
+      <c r="AA7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB7" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
@@ -1223,14 +1191,14 @@
       <c r="X8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Y8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB8" s="8" t="s">
-        <v>37</v>
+      <c r="Y8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB8" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
@@ -1311,13 +1279,13 @@
         <v>22</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB9" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="AA9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB9" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
@@ -1343,7 +1311,7 @@
       <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1355,22 +1323,22 @@
       <c r="J10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P10" s="7" t="s">
+      <c r="K10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P10" s="6" t="s">
         <v>14</v>
       </c>
       <c r="Q10" s="3" t="s">
@@ -1379,7 +1347,7 @@
       <c r="R10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="S10" s="6" t="s">
+      <c r="S10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="T10" s="2" t="s">
@@ -1400,11 +1368,11 @@
       <c r="Y10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AA10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB10" s="8" t="s">
-        <v>39</v>
+      <c r="AA10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB10" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
@@ -1442,22 +1410,22 @@
       <c r="J11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P11" s="7" t="s">
+      <c r="K11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="Q11" s="3" t="s">
@@ -1487,11 +1455,11 @@
       <c r="Y11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AA11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB11" s="8" t="s">
-        <v>40</v>
+      <c r="AA11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB11" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
@@ -1508,7 +1476,7 @@
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -1529,22 +1497,22 @@
       <c r="J12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P12" s="7" t="s">
+      <c r="K12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="Q12" s="3" t="s">
@@ -1574,11 +1542,11 @@
       <c r="Y12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AA12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB12" s="8" t="s">
-        <v>41</v>
+      <c r="AA12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB12" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
@@ -1587,7 +1555,7 @@
     </row>
     <row r="13" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>22</v>
@@ -1616,28 +1584,28 @@
       <c r="J13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P13" s="7" t="s">
+      <c r="K13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R13" s="6" t="s">
+      <c r="R13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="S13" s="2" t="s">
@@ -1661,11 +1629,11 @@
       <c r="Y13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AA13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB13" s="8" t="s">
-        <v>42</v>
+      <c r="AA13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB13" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
@@ -1676,7 +1644,7 @@
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1703,28 +1671,28 @@
       <c r="J14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P14" s="7" t="s">
+      <c r="K14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P14" s="6" t="s">
         <v>14</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R14" s="6" t="s">
+      <c r="R14" s="5" t="s">
         <v>8</v>
       </c>
       <c r="S14" s="2" t="s">
@@ -1748,12 +1716,8 @@
       <c r="Y14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AA14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB14" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
@@ -1790,22 +1754,22 @@
       <c r="J15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P15" s="7" t="s">
+      <c r="K15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P15" s="6" t="s">
         <v>14</v>
       </c>
       <c r="Q15" s="3" t="s">
@@ -1867,22 +1831,22 @@
       <c r="J16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P16" s="7" t="s">
+      <c r="K16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P16" s="6" t="s">
         <v>14</v>
       </c>
       <c r="Q16" s="3" t="s">
@@ -1929,7 +1893,7 @@
       <c r="E17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -2021,7 +1985,7 @@
       <c r="J18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="K18" s="5" t="s">
         <v>13</v>
       </c>
       <c r="L18" s="2" t="s">
@@ -2036,7 +2000,7 @@
       <c r="O18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P18" s="6" t="s">
+      <c r="P18" s="5" t="s">
         <v>13</v>
       </c>
       <c r="Q18" s="2" t="s">
@@ -2064,12 +2028,12 @@
         <v>22</v>
       </c>
       <c r="Y18" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A19" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>22</v>
@@ -2145,8 +2109,8 @@
       </c>
     </row>
     <row r="20" spans="1:25" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A20" s="5" t="s">
-        <v>26</v>
+      <c r="A20" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>22</v>
@@ -2205,7 +2169,7 @@
       <c r="T20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="U20" s="6" t="s">
+      <c r="U20" s="5" t="s">
         <v>11</v>
       </c>
       <c r="V20" s="2" t="s">
@@ -2218,7 +2182,7 @@
         <v>10</v>
       </c>
       <c r="Y20" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
@@ -2237,8 +2201,8 @@
       <c r="E21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>44</v>
+      <c r="F21" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>22</v>
@@ -2508,7 +2472,7 @@
         <v>22</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="T24" s="2" t="s">
         <v>10</v>
@@ -2552,16 +2516,16 @@
         <v>15</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>12</v>
@@ -2575,17 +2539,17 @@
       <c r="O25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P25" s="5" t="s">
-        <v>28</v>
+      <c r="P25" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="T25" s="2" t="s">
         <v>10</v>

</xml_diff>